<commit_message>
Netzplan Übung 2 (FIAE D)
</commit_message>
<xml_diff>
--- a/FIAEB Übungen/Netzplan_Übung2.xlsx
+++ b/FIAEB Übungen/Netzplan_Übung2.xlsx
@@ -734,13 +734,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>259200</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>161640</xdr:rowOff>
+      <xdr:rowOff>162000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>271080</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -749,7 +749,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1070640" y="3265560"/>
+          <a:off x="1070640" y="3265920"/>
           <a:ext cx="282240" cy="1800"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -902,13 +902,13 @@
       <xdr:col>18</xdr:col>
       <xdr:colOff>720</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>152640</xdr:rowOff>
+      <xdr:rowOff>153000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>271080</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -917,7 +917,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4869720" y="3256560"/>
+          <a:off x="4869720" y="3256920"/>
           <a:ext cx="1622880" cy="11160"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1337,7 +1337,7 @@
       <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="3.83"/>
   </cols>
@@ -2451,7 +2451,7 @@
       <selection pane="topLeft" activeCell="T10" activeCellId="0" sqref="T10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="3.83"/>
   </cols>

</xml_diff>